<commit_message>
Ajout de la presentation et modification du cahier des charges
</commit_message>
<xml_diff>
--- a/Remises/Revue2/CahierCharge-002.xlsx
+++ b/Remises/Revue2/CahierCharge-002.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
   <si>
     <t>Spécification</t>
   </si>
@@ -294,157 +293,22 @@
     <t>Être stereo</t>
   </si>
   <si>
-    <t>Interface</t>
-  </si>
-  <si>
-    <t>Modif UML</t>
-  </si>
-  <si>
-    <t>Écran</t>
-  </si>
-  <si>
-    <t>Boutons</t>
-  </si>
-  <si>
-    <t>Enregistrement</t>
-  </si>
-  <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>DAC</t>
-  </si>
-  <si>
-    <t>EQ (filtres)</t>
-  </si>
-  <si>
-    <t>Ajustement volume</t>
-  </si>
-  <si>
-    <t>Harmonizer</t>
-  </si>
-  <si>
-    <t>Écran tactile</t>
-  </si>
-  <si>
-    <t>Modification</t>
-  </si>
-  <si>
-    <t>Conditionnement</t>
-  </si>
-  <si>
-    <t>Schema bloc traitement de signal</t>
-  </si>
-  <si>
-    <t>Traitement de signal</t>
-  </si>
-  <si>
-    <t>Autocorrélation</t>
-  </si>
-  <si>
-    <t>Ordinogramme</t>
-  </si>
-  <si>
-    <t>15 mars</t>
-  </si>
-  <si>
-    <t>1er mars</t>
-  </si>
-  <si>
-    <t>Mettre à jour le cahier des charges</t>
-  </si>
-  <si>
-    <t>Schéma matériel final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UML corrigé </t>
-  </si>
-  <si>
-    <t>5 avril</t>
-  </si>
-  <si>
-    <t>Filtres</t>
-  </si>
-  <si>
-    <t>Démo 1</t>
-  </si>
-  <si>
-    <t>16 avril</t>
-  </si>
-  <si>
-    <t>Interface (menu)</t>
-  </si>
-  <si>
-    <t>Communication série</t>
-  </si>
-  <si>
     <t>Revue 2</t>
   </si>
   <si>
-    <t>Demo 2</t>
-  </si>
-  <si>
-    <t>Demo 3</t>
-  </si>
-  <si>
-    <t>22 février</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1er mars </t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>CODEC + EMIF</t>
-  </si>
-  <si>
-    <t>Bande de fréquence</t>
-  </si>
-  <si>
-    <t>Modification des fréquences</t>
-  </si>
-  <si>
-    <t>Sommation des bandes</t>
-  </si>
-  <si>
-    <t>22 mars</t>
-  </si>
-  <si>
-    <t>29 mars</t>
-  </si>
-  <si>
-    <t>Écran LCD + touches</t>
-  </si>
-  <si>
-    <t>Ajustement de volume</t>
-  </si>
-  <si>
-    <t>Prévision</t>
-  </si>
-  <si>
-    <t>25 février</t>
-  </si>
-  <si>
-    <t>17 février</t>
-  </si>
-  <si>
-    <t>14 mars</t>
-  </si>
-  <si>
-    <t>18 mars</t>
-  </si>
-  <si>
-    <t>25 mars</t>
-  </si>
-  <si>
-    <t>2 avril</t>
-  </si>
-  <si>
-    <t>8 avril</t>
-  </si>
-  <si>
-    <t>Intégration</t>
+    <t>Fcont7</t>
+  </si>
+  <si>
+    <t>Respecter le budget estimé</t>
+  </si>
+  <si>
+    <t>Prix total du projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matériel : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heures : </t>
   </si>
 </sst>
 </file>
@@ -689,14 +553,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -710,6 +569,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1035,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,7 +919,7 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1084,10 +946,10 @@
       <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1108,8 +970,8 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="36"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15" t="s">
         <v>45</v>
       </c>
@@ -1128,8 +990,8 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="36"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="30" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1150,8 +1012,8 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15" t="s">
         <v>46</v>
       </c>
@@ -1170,7 +1032,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="37"/>
-      <c r="B8" s="34"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
@@ -1241,10 +1103,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1259,8 +1121,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="12" t="s">
         <v>55</v>
       </c>
@@ -1275,8 +1137,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="12" t="s">
         <v>56</v>
       </c>
@@ -1291,10 +1153,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -1309,8 +1171,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="12" t="s">
         <v>65</v>
       </c>
@@ -1343,10 +1205,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -1363,8 +1225,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="14" t="s">
         <v>32</v>
       </c>
@@ -1393,10 +1255,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="25" t="s">
@@ -1411,8 +1273,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="25" t="s">
         <v>87</v>
       </c>
@@ -1421,10 +1283,10 @@
       <c r="F22" s="26"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1439,8 +1301,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="26" t="s">
         <v>88</v>
       </c>
@@ -1501,8 +1363,42 @@
         <v>36</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C4:C5"/>
@@ -1520,353 +1416,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L29"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="9" max="9" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K3" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="L3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" t="s">
-        <v>102</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I6" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="K6" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I7" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I8" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="L8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="L9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" t="s">
-        <v>105</v>
-      </c>
-      <c r="J10" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="L10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>96</v>
-      </c>
-      <c r="I13" t="s">
-        <v>108</v>
-      </c>
-      <c r="J13" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="K13" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>97</v>
-      </c>
-      <c r="I14" t="s">
-        <v>109</v>
-      </c>
-      <c r="J14" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="K14" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="L14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" t="s">
-        <v>110</v>
-      </c>
-      <c r="J15" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="K15" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="L15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="H17" t="s">
-        <v>118</v>
-      </c>
-      <c r="I17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I19" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="K19" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="L19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I20" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="J20" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="K20" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="L20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I21" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="L21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="H23" t="s">
-        <v>119</v>
-      </c>
-      <c r="I23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I25" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="J25" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="K25" t="s">
-        <v>120</v>
-      </c>
-      <c r="L25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I26" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="J26" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="K26" t="s">
-        <v>114</v>
-      </c>
-      <c r="L26">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>90</v>
-      </c>
-      <c r="I27" t="s">
-        <v>116</v>
-      </c>
-      <c r="J27" t="s">
-        <v>132</v>
-      </c>
-      <c r="K27" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="L27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I29" t="s">
-        <v>139</v>
-      </c>
-      <c r="J29" t="s">
-        <v>138</v>
-      </c>
-      <c r="K29" t="s">
-        <v>114</v>
-      </c>
-      <c r="L29">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour du cahier des charges
</commit_message>
<xml_diff>
--- a/Remises/Revue2/CahierCharge-002.xlsx
+++ b/Remises/Revue2/CahierCharge-002.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\Sessions\S5\Projet\Git\Remises\Revue2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSITÉ\S5\Projet\Git\Remises\Revue2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,12 +224,6 @@
     <t>Ressemblance du contenu spectral</t>
   </si>
   <si>
-    <t>Pouvoir accueillir une guitare ou un micro</t>
-  </si>
-  <si>
-    <t>Jack 1/4"</t>
-  </si>
-  <si>
     <t>Jack 3.5mm</t>
   </si>
   <si>
@@ -305,10 +299,16 @@
     <t>Prix total du projet</t>
   </si>
   <si>
-    <t xml:space="preserve">Matériel : </t>
-  </si>
-  <si>
     <t xml:space="preserve">Heures : </t>
+  </si>
+  <si>
+    <t>Pouvoir accueillir un micro</t>
+  </si>
+  <si>
+    <t>Jack 3,5mm</t>
+  </si>
+  <si>
+    <t>Matériel : 330</t>
   </si>
 </sst>
 </file>
@@ -556,6 +556,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -569,9 +572,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -601,7 +601,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -899,19 +899,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -919,10 +919,10 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -942,14 +942,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -968,10 +968,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="15" t="s">
         <v>45</v>
       </c>
@@ -988,10 +988,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="31" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1010,10 +1010,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="15" t="s">
         <v>46</v>
       </c>
@@ -1030,9 +1030,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
-      <c r="B8" s="33"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>50</v>
@@ -1066,63 +1066,63 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>80</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="32" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="12" t="s">
         <v>55</v>
       </c>
@@ -1136,9 +1136,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="12" t="s">
         <v>56</v>
       </c>
@@ -1152,11 +1152,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -1170,9 +1170,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
-      <c r="B16" s="33"/>
+    <row r="16" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="12" t="s">
         <v>65</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>51</v>
@@ -1204,11 +1204,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="31" t="s">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -1224,9 +1224,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="14" t="s">
         <v>32</v>
       </c>
@@ -1234,9 +1234,9 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>21</v>
@@ -1245,7 +1245,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>51</v>
@@ -1254,63 +1254,63 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="34" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="29" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="29" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1318,17 +1318,17 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -1336,56 +1336,56 @@
         <v>29</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="34" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>92</v>
-      </c>
       <c r="D28" s="27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F28" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>64</v>
@@ -1396,11 +1396,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B12:B14"/>
@@ -1413,6 +1408,11 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update cahier de charge -002
</commit_message>
<xml_diff>
--- a/Remises/Revue2/CahierCharge-002.xlsx
+++ b/Remises/Revue2/CahierCharge-002.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSITÉ\S5\Projet\Git\Remises\Revue2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\Sessions\S5\Projet\Git\Remises\Revue2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
   <si>
     <t>Spécification</t>
   </si>
@@ -309,6 +309,21 @@
   </si>
   <si>
     <t>Matériel : 330</t>
+  </si>
+  <si>
+    <t>Afficher l'erreur sur l'accordement d'une note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de note </t>
+  </si>
+  <si>
+    <t>Précision de l'accordement</t>
+  </si>
+  <si>
+    <t>+/-2%</t>
+  </si>
+  <si>
+    <t>Fsec8</t>
   </si>
 </sst>
 </file>
@@ -474,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -556,9 +571,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -574,6 +586,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -581,6 +596,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -601,7 +619,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -897,21 +915,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -922,7 +940,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -942,14 +960,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -968,10 +986,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="36"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="15" t="s">
         <v>45</v>
       </c>
@@ -988,10 +1006,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="36"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="30" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1010,10 +1028,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="15" t="s">
         <v>46</v>
       </c>
@@ -1030,9 +1048,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="37"/>
-      <c r="B8" s="34"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
@@ -1046,7 +1064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1066,7 +1084,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>11</v>
       </c>
@@ -1084,7 +1102,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>12</v>
       </c>
@@ -1102,11 +1120,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1120,9 +1138,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="12" t="s">
         <v>55</v>
       </c>
@@ -1136,9 +1154,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="12" t="s">
         <v>56</v>
       </c>
@@ -1152,11 +1170,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -1170,9 +1188,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="34"/>
+    <row r="16" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="12" t="s">
         <v>65</v>
       </c>
@@ -1184,235 +1202,271 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="38">
+        <v>6</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E19" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="32" t="s">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E20" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="14" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B23" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C23" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="26" t="s">
-        <v>86</v>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>24</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>34</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>74</v>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>73</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B30" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C30" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D30" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F30" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="27" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E31" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F31" s="27" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>